<commit_message>
fix some bugs for uploadController and excelParser for courses and recommendations
</commit_message>
<xml_diff>
--- a/backend/src/uploads/files/sp25-candidatelist 2.xlsx
+++ b/backend/src/uploads/files/sp25-candidatelist 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jasontran2048\UTD-Projects\Senior\S25\grader-assignment-system\backend\src\uploads\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\MSCS\TA\CS Project\GAS\Final_Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0239DF3E-8481-4B62-B39D-F111041C544F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5446BE3-295C-4958-A390-15CF31190DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2670" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - application_download2" sheetId="1" r:id="rId1"/>
@@ -6571,37 +6571,37 @@
   <dimension ref="A1:V304"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="S308" sqref="S307:S308"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="19.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.28515625" style="1" customWidth="1"/>
-    <col min="24" max="27" width="8.28515625" style="1"/>
-    <col min="28" max="28" width="15.7109375" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="8.28515625" style="1"/>
+    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="58" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14" style="1" customWidth="1"/>
+    <col min="16" max="16" width="29.44140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="29.44140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="24.109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.77734375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.77734375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="8.33203125" style="1" customWidth="1"/>
+    <col min="24" max="27" width="8.33203125" style="1"/>
+    <col min="28" max="28" width="15.6640625" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="27.75" customHeight="1">
@@ -6764,7 +6764,7 @@
         <v>559042</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="4" spans="1:22" ht="19.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>1442</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>559084</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="5" spans="1:22" ht="19.95" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>1443</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v>559012</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="6" spans="1:22" ht="19.95" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>1444</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>559272</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="7" spans="1:22" ht="19.95" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>1445</v>
       </c>
@@ -7028,7 +7028,7 @@
         <v>559160</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="8" spans="1:22" ht="19.95" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>1446</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>559096</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="9" spans="1:22" ht="19.95" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>1447</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>559260</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="10" spans="1:22" ht="19.95" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>1448</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>559276</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="11" spans="1:22" ht="19.95" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>1449</v>
       </c>
@@ -7292,7 +7292,7 @@
         <v>559069</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="12" spans="1:22" ht="19.95" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>1450</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>559010</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="13" spans="1:22" ht="19.95" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>1451</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>559046</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="14" spans="1:22" ht="19.95" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>1452</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>559014</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="15" spans="1:22" ht="19.95" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>1453</v>
       </c>
@@ -7556,7 +7556,7 @@
         <v>559290</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="16" spans="1:22" ht="19.95" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>1454</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>559230</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="17" spans="1:22" ht="19.95" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>1455</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>559060</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="18" spans="1:22" ht="19.95" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>1456</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>559201</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="19" spans="1:22" ht="19.95" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>1457</v>
       </c>
@@ -7820,7 +7820,7 @@
         <v>559044</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="20" spans="1:22" ht="19.95" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>1458</v>
       </c>
@@ -7886,7 +7886,7 @@
         <v>559204</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="21" spans="1:22" ht="19.95" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>1459</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>559097</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="22" spans="1:22" ht="19.95" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>1460</v>
       </c>
@@ -8018,7 +8018,7 @@
         <v>559226</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="23" spans="1:22" ht="19.95" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>1461</v>
       </c>
@@ -8084,7 +8084,7 @@
         <v>559036</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="24" spans="1:22" ht="19.95" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>1462</v>
       </c>
@@ -8150,7 +8150,7 @@
         <v>559091</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="25" spans="1:22" ht="19.95" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>1463</v>
       </c>
@@ -8216,7 +8216,7 @@
         <v>559293</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="26" spans="1:22" ht="19.95" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>1464</v>
       </c>
@@ -8282,7 +8282,7 @@
         <v>559071</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="27" spans="1:22" ht="19.95" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>1465</v>
       </c>
@@ -8348,7 +8348,7 @@
         <v>559138</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="28" spans="1:22" ht="19.95" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>1466</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>559038</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="29" spans="1:22" ht="19.95" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>1467</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>559056</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="30" spans="1:22" ht="19.95" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>1468</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>559182</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="31" spans="1:22" ht="19.95" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>1469</v>
       </c>
@@ -8610,7 +8610,7 @@
         <v>559256</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="32" spans="1:22" ht="19.95" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>1470</v>
       </c>
@@ -8676,7 +8676,7 @@
         <v>559074</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="33" spans="1:22" ht="19.95" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>1471</v>
       </c>
@@ -8742,7 +8742,7 @@
         <v>559212</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="34" spans="1:22" ht="19.95" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>1472</v>
       </c>
@@ -8808,7 +8808,7 @@
         <v>559176</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="35" spans="1:22" ht="19.95" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>1473</v>
       </c>
@@ -8874,7 +8874,7 @@
         <v>559220</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="36" spans="1:22" ht="19.95" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>1474</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>559227</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="37" spans="1:22" ht="19.95" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>1475</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>559288</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="38" spans="1:22" ht="19.95" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>1476</v>
       </c>
@@ -9070,7 +9070,7 @@
         <v>559216</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="39" spans="1:22" ht="19.95" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>1477</v>
       </c>
@@ -9136,7 +9136,7 @@
         <v>559099</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="40" spans="1:22" ht="19.95" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>1478</v>
       </c>
@@ -9202,7 +9202,7 @@
         <v>559231</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="41" spans="1:22" ht="19.95" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>1479</v>
       </c>
@@ -9266,7 +9266,7 @@
         <v>559259</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="42" spans="1:22" ht="19.95" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>1480</v>
       </c>
@@ -9332,7 +9332,7 @@
         <v>559085</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="43" spans="1:22" ht="19.95" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>1481</v>
       </c>
@@ -9398,7 +9398,7 @@
         <v>559236</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="44" spans="1:22" ht="19.95" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>1482</v>
       </c>
@@ -9464,7 +9464,7 @@
         <v>559052</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="45" spans="1:22" ht="19.95" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>1483</v>
       </c>
@@ -9530,7 +9530,7 @@
         <v>559020</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="46" spans="1:22" ht="19.95" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>1484</v>
       </c>
@@ -9596,7 +9596,7 @@
         <v>559047</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="47" spans="1:22" ht="19.95" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>1485</v>
       </c>
@@ -9662,7 +9662,7 @@
         <v>559183</v>
       </c>
     </row>
-    <row r="48" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="48" spans="1:22" ht="19.95" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>1486</v>
       </c>
@@ -9728,7 +9728,7 @@
         <v>559102</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="49" spans="1:22" ht="19.95" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>1487</v>
       </c>
@@ -9794,7 +9794,7 @@
         <v>559295</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="50" spans="1:22" ht="19.95" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>1488</v>
       </c>
@@ -9860,7 +9860,7 @@
         <v>559065</v>
       </c>
     </row>
-    <row r="51" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="51" spans="1:22" ht="19.95" customHeight="1">
       <c r="A51" s="1" t="s">
         <v>1489</v>
       </c>
@@ -9926,7 +9926,7 @@
         <v>559103</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="52" spans="1:22" ht="19.95" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>1490</v>
       </c>
@@ -9992,7 +9992,7 @@
         <v>559258</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="53" spans="1:22" ht="19.95" customHeight="1">
       <c r="A53" s="1" t="s">
         <v>1491</v>
       </c>
@@ -10058,7 +10058,7 @@
         <v>559159</v>
       </c>
     </row>
-    <row r="54" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="54" spans="1:22" ht="19.95" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>1492</v>
       </c>
@@ -10124,7 +10124,7 @@
         <v>559239</v>
       </c>
     </row>
-    <row r="55" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="55" spans="1:22" ht="19.95" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>1493</v>
       </c>
@@ -10190,7 +10190,7 @@
         <v>559271</v>
       </c>
     </row>
-    <row r="56" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="56" spans="1:22" ht="19.95" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>1494</v>
       </c>
@@ -10256,7 +10256,7 @@
         <v>559051</v>
       </c>
     </row>
-    <row r="57" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="57" spans="1:22" ht="19.95" customHeight="1">
       <c r="A57" s="1" t="s">
         <v>1495</v>
       </c>
@@ -10322,7 +10322,7 @@
         <v>559233</v>
       </c>
     </row>
-    <row r="58" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="58" spans="1:22" ht="19.95" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>1496</v>
       </c>
@@ -10388,7 +10388,7 @@
         <v>559165</v>
       </c>
     </row>
-    <row r="59" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="59" spans="1:22" ht="19.95" customHeight="1">
       <c r="A59" s="1" t="s">
         <v>1497</v>
       </c>
@@ -10454,7 +10454,7 @@
         <v>559264</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="60" spans="1:22" ht="19.95" customHeight="1">
       <c r="A60" s="1" t="s">
         <v>1498</v>
       </c>
@@ -10520,7 +10520,7 @@
         <v>559115</v>
       </c>
     </row>
-    <row r="61" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="61" spans="1:22" ht="19.95" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>1499</v>
       </c>
@@ -10586,7 +10586,7 @@
         <v>559025</v>
       </c>
     </row>
-    <row r="62" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="62" spans="1:22" ht="19.95" customHeight="1">
       <c r="A62" s="1" t="s">
         <v>1500</v>
       </c>
@@ -10652,7 +10652,7 @@
         <v>559155</v>
       </c>
     </row>
-    <row r="63" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="63" spans="1:22" ht="19.95" customHeight="1">
       <c r="A63" s="1" t="s">
         <v>1501</v>
       </c>
@@ -10718,7 +10718,7 @@
         <v>559021</v>
       </c>
     </row>
-    <row r="64" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="64" spans="1:22" ht="19.95" customHeight="1">
       <c r="A64" s="1" t="s">
         <v>1502</v>
       </c>
@@ -10784,7 +10784,7 @@
         <v>559157</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="65" spans="1:22" ht="19.95" customHeight="1">
       <c r="A65" s="1" t="s">
         <v>1503</v>
       </c>
@@ -10850,7 +10850,7 @@
         <v>559177</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="66" spans="1:22" ht="19.95" customHeight="1">
       <c r="A66" s="1" t="s">
         <v>1504</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>559105</v>
       </c>
     </row>
-    <row r="67" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="67" spans="1:22" ht="19.95" customHeight="1">
       <c r="A67" s="1" t="s">
         <v>1505</v>
       </c>
@@ -10982,7 +10982,7 @@
         <v>559087</v>
       </c>
     </row>
-    <row r="68" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="68" spans="1:22" ht="19.95" customHeight="1">
       <c r="A68" s="1" t="s">
         <v>1506</v>
       </c>
@@ -11048,7 +11048,7 @@
         <v>559218</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="69" spans="1:22" ht="19.95" customHeight="1">
       <c r="A69" s="1" t="s">
         <v>1507</v>
       </c>
@@ -11114,7 +11114,7 @@
         <v>559062</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="70" spans="1:22" ht="19.95" customHeight="1">
       <c r="A70" s="1" t="s">
         <v>1508</v>
       </c>
@@ -11180,7 +11180,7 @@
         <v>559179</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="71" spans="1:22" ht="19.95" customHeight="1">
       <c r="A71" s="1" t="s">
         <v>1509</v>
       </c>
@@ -11246,7 +11246,7 @@
         <v>559004</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="72" spans="1:22" ht="19.95" customHeight="1">
       <c r="A72" s="1" t="s">
         <v>1510</v>
       </c>
@@ -11312,7 +11312,7 @@
         <v>559198</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="73" spans="1:22" ht="19.95" customHeight="1">
       <c r="A73" s="1" t="s">
         <v>1511</v>
       </c>
@@ -11378,7 +11378,7 @@
         <v>559127</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="74" spans="1:22" ht="19.95" customHeight="1">
       <c r="A74" s="1" t="s">
         <v>1512</v>
       </c>
@@ -11444,7 +11444,7 @@
         <v>559080</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="75" spans="1:22" ht="19.95" customHeight="1">
       <c r="A75" s="1" t="s">
         <v>1513</v>
       </c>
@@ -11510,7 +11510,7 @@
         <v>559154</v>
       </c>
     </row>
-    <row r="76" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="76" spans="1:22" ht="19.95" customHeight="1">
       <c r="A76" s="1" t="s">
         <v>1514</v>
       </c>
@@ -11576,7 +11576,7 @@
         <v>559245</v>
       </c>
     </row>
-    <row r="77" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="77" spans="1:22" ht="19.95" customHeight="1">
       <c r="A77" s="1" t="s">
         <v>1515</v>
       </c>
@@ -11642,7 +11642,7 @@
         <v>559124</v>
       </c>
     </row>
-    <row r="78" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="78" spans="1:22" ht="19.95" customHeight="1">
       <c r="A78" s="1" t="s">
         <v>1516</v>
       </c>
@@ -11708,7 +11708,7 @@
         <v>559017</v>
       </c>
     </row>
-    <row r="79" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="79" spans="1:22" ht="19.95" customHeight="1">
       <c r="A79" s="1" t="s">
         <v>1517</v>
       </c>
@@ -11774,7 +11774,7 @@
         <v>559187</v>
       </c>
     </row>
-    <row r="80" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="80" spans="1:22" ht="19.95" customHeight="1">
       <c r="A80" s="1" t="s">
         <v>1518</v>
       </c>
@@ -11840,7 +11840,7 @@
         <v>559291</v>
       </c>
     </row>
-    <row r="81" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="81" spans="1:22" ht="19.95" customHeight="1">
       <c r="A81" s="1" t="s">
         <v>1519</v>
       </c>
@@ -11906,7 +11906,7 @@
         <v>559135</v>
       </c>
     </row>
-    <row r="82" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="82" spans="1:22" ht="19.95" customHeight="1">
       <c r="A82" s="1" t="s">
         <v>1520</v>
       </c>
@@ -11972,7 +11972,7 @@
         <v>559126</v>
       </c>
     </row>
-    <row r="83" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="83" spans="1:22" ht="19.95" customHeight="1">
       <c r="A83" s="1" t="s">
         <v>1521</v>
       </c>
@@ -12038,7 +12038,7 @@
         <v>559024</v>
       </c>
     </row>
-    <row r="84" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="84" spans="1:22" ht="19.95" customHeight="1">
       <c r="A84" s="1" t="s">
         <v>1522</v>
       </c>
@@ -12104,7 +12104,7 @@
         <v>559082</v>
       </c>
     </row>
-    <row r="85" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="85" spans="1:22" ht="19.95" customHeight="1">
       <c r="A85" s="1" t="s">
         <v>1523</v>
       </c>
@@ -12168,7 +12168,7 @@
         <v>559140</v>
       </c>
     </row>
-    <row r="86" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="86" spans="1:22" ht="19.95" customHeight="1">
       <c r="A86" s="1" t="s">
         <v>1524</v>
       </c>
@@ -12234,7 +12234,7 @@
         <v>559270</v>
       </c>
     </row>
-    <row r="87" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="87" spans="1:22" ht="19.95" customHeight="1">
       <c r="A87" s="1" t="s">
         <v>1525</v>
       </c>
@@ -12300,7 +12300,7 @@
         <v>559009</v>
       </c>
     </row>
-    <row r="88" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="88" spans="1:22" ht="19.95" customHeight="1">
       <c r="A88" s="1" t="s">
         <v>1526</v>
       </c>
@@ -12366,7 +12366,7 @@
         <v>559121</v>
       </c>
     </row>
-    <row r="89" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="89" spans="1:22" ht="19.95" customHeight="1">
       <c r="A89" s="1" t="s">
         <v>1527</v>
       </c>
@@ -12432,7 +12432,7 @@
         <v>559244</v>
       </c>
     </row>
-    <row r="90" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="90" spans="1:22" ht="19.95" customHeight="1">
       <c r="A90" s="1" t="s">
         <v>1528</v>
       </c>
@@ -12498,7 +12498,7 @@
         <v>559275</v>
       </c>
     </row>
-    <row r="91" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="91" spans="1:22" ht="19.95" customHeight="1">
       <c r="A91" s="1" t="s">
         <v>1529</v>
       </c>
@@ -12564,7 +12564,7 @@
         <v>559139</v>
       </c>
     </row>
-    <row r="92" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="92" spans="1:22" ht="19.95" customHeight="1">
       <c r="A92" s="1" t="s">
         <v>1530</v>
       </c>
@@ -12630,7 +12630,7 @@
         <v>559186</v>
       </c>
     </row>
-    <row r="93" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="93" spans="1:22" ht="19.95" customHeight="1">
       <c r="A93" s="1" t="s">
         <v>1531</v>
       </c>
@@ -12696,7 +12696,7 @@
         <v>559151</v>
       </c>
     </row>
-    <row r="94" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="94" spans="1:22" ht="19.95" customHeight="1">
       <c r="A94" s="1" t="s">
         <v>1532</v>
       </c>
@@ -12762,7 +12762,7 @@
         <v>559002</v>
       </c>
     </row>
-    <row r="95" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="95" spans="1:22" ht="19.95" customHeight="1">
       <c r="A95" s="1" t="s">
         <v>1533</v>
       </c>
@@ -12828,7 +12828,7 @@
         <v>559057</v>
       </c>
     </row>
-    <row r="96" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="96" spans="1:22" ht="19.95" customHeight="1">
       <c r="A96" s="1" t="s">
         <v>1534</v>
       </c>
@@ -12894,7 +12894,7 @@
         <v>559148</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="97" spans="1:22" ht="19.95" customHeight="1">
       <c r="A97" s="1" t="s">
         <v>1535</v>
       </c>
@@ -12960,7 +12960,7 @@
         <v>559106</v>
       </c>
     </row>
-    <row r="98" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="98" spans="1:22" ht="19.95" customHeight="1">
       <c r="A98" s="1" t="s">
         <v>1536</v>
       </c>
@@ -13026,7 +13026,7 @@
         <v>559238</v>
       </c>
     </row>
-    <row r="99" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="99" spans="1:22" ht="19.95" customHeight="1">
       <c r="A99" s="1" t="s">
         <v>1537</v>
       </c>
@@ -13092,7 +13092,7 @@
         <v>559296</v>
       </c>
     </row>
-    <row r="100" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="100" spans="1:22" ht="19.95" customHeight="1">
       <c r="A100" s="1" t="s">
         <v>1538</v>
       </c>
@@ -13158,7 +13158,7 @@
         <v>559114</v>
       </c>
     </row>
-    <row r="101" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="101" spans="1:22" ht="19.95" customHeight="1">
       <c r="A101" s="1" t="s">
         <v>1539</v>
       </c>
@@ -13224,7 +13224,7 @@
         <v>559184</v>
       </c>
     </row>
-    <row r="102" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="102" spans="1:22" ht="19.95" customHeight="1">
       <c r="A102" s="1" t="s">
         <v>1540</v>
       </c>
@@ -13290,7 +13290,7 @@
         <v>559156</v>
       </c>
     </row>
-    <row r="103" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="103" spans="1:22" ht="19.95" customHeight="1">
       <c r="A103" s="1" t="s">
         <v>1541</v>
       </c>
@@ -13356,7 +13356,7 @@
         <v>559294</v>
       </c>
     </row>
-    <row r="104" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="104" spans="1:22" ht="19.95" customHeight="1">
       <c r="A104" s="1" t="s">
         <v>1542</v>
       </c>
@@ -13422,7 +13422,7 @@
         <v>559248</v>
       </c>
     </row>
-    <row r="105" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="105" spans="1:22" ht="19.95" customHeight="1">
       <c r="A105" s="1" t="s">
         <v>1543</v>
       </c>
@@ -13488,7 +13488,7 @@
         <v>559152</v>
       </c>
     </row>
-    <row r="106" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="106" spans="1:22" ht="19.95" customHeight="1">
       <c r="A106" s="1" t="s">
         <v>1544</v>
       </c>
@@ -13554,7 +13554,7 @@
         <v>559277</v>
       </c>
     </row>
-    <row r="107" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="107" spans="1:22" ht="19.95" customHeight="1">
       <c r="A107" s="1" t="s">
         <v>1545</v>
       </c>
@@ -13620,7 +13620,7 @@
         <v>559145</v>
       </c>
     </row>
-    <row r="108" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="108" spans="1:22" ht="19.95" customHeight="1">
       <c r="A108" s="1" t="s">
         <v>1546</v>
       </c>
@@ -13686,7 +13686,7 @@
         <v>559136</v>
       </c>
     </row>
-    <row r="109" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="109" spans="1:22" ht="19.95" customHeight="1">
       <c r="A109" s="1" t="s">
         <v>1547</v>
       </c>
@@ -13752,7 +13752,7 @@
         <v>559283</v>
       </c>
     </row>
-    <row r="110" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="110" spans="1:22" ht="19.95" customHeight="1">
       <c r="A110" s="1" t="s">
         <v>1548</v>
       </c>
@@ -13818,7 +13818,7 @@
         <v>559251</v>
       </c>
     </row>
-    <row r="111" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="111" spans="1:22" ht="19.95" customHeight="1">
       <c r="A111" s="1" t="s">
         <v>1549</v>
       </c>
@@ -13882,7 +13882,7 @@
         <v>559016</v>
       </c>
     </row>
-    <row r="112" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="112" spans="1:22" ht="19.95" customHeight="1">
       <c r="A112" s="1" t="s">
         <v>1550</v>
       </c>
@@ -13948,7 +13948,7 @@
         <v>559278</v>
       </c>
     </row>
-    <row r="113" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="113" spans="1:22" ht="19.95" customHeight="1">
       <c r="A113" s="1" t="s">
         <v>1551</v>
       </c>
@@ -14014,7 +14014,7 @@
         <v>559171</v>
       </c>
     </row>
-    <row r="114" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="114" spans="1:22" ht="19.95" customHeight="1">
       <c r="A114" s="1" t="s">
         <v>1552</v>
       </c>
@@ -14080,7 +14080,7 @@
         <v>559265</v>
       </c>
     </row>
-    <row r="115" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="115" spans="1:22" ht="19.95" customHeight="1">
       <c r="A115" s="1" t="s">
         <v>1553</v>
       </c>
@@ -14146,7 +14146,7 @@
         <v>559150</v>
       </c>
     </row>
-    <row r="116" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="116" spans="1:22" ht="19.95" customHeight="1">
       <c r="A116" s="1" t="s">
         <v>1554</v>
       </c>
@@ -14212,7 +14212,7 @@
         <v>559098</v>
       </c>
     </row>
-    <row r="117" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="117" spans="1:22" ht="19.95" customHeight="1">
       <c r="A117" s="1" t="s">
         <v>1555</v>
       </c>
@@ -14278,7 +14278,7 @@
         <v>559093</v>
       </c>
     </row>
-    <row r="118" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="118" spans="1:22" ht="19.95" customHeight="1">
       <c r="A118" s="1" t="s">
         <v>1556</v>
       </c>
@@ -14342,7 +14342,7 @@
         <v>559067</v>
       </c>
     </row>
-    <row r="119" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="119" spans="1:22" ht="19.95" customHeight="1">
       <c r="A119" s="1" t="s">
         <v>1557</v>
       </c>
@@ -14408,7 +14408,7 @@
         <v>559167</v>
       </c>
     </row>
-    <row r="120" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="120" spans="1:22" ht="19.95" customHeight="1">
       <c r="A120" s="1" t="s">
         <v>1558</v>
       </c>
@@ -14474,7 +14474,7 @@
         <v>559209</v>
       </c>
     </row>
-    <row r="121" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="121" spans="1:22" ht="19.95" customHeight="1">
       <c r="A121" s="1" t="s">
         <v>1559</v>
       </c>
@@ -14540,7 +14540,7 @@
         <v>559011</v>
       </c>
     </row>
-    <row r="122" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="122" spans="1:22" ht="19.95" customHeight="1">
       <c r="A122" s="1" t="s">
         <v>1560</v>
       </c>
@@ -14606,7 +14606,7 @@
         <v>559032</v>
       </c>
     </row>
-    <row r="123" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="123" spans="1:22" ht="19.95" customHeight="1">
       <c r="A123" s="1" t="s">
         <v>1561</v>
       </c>
@@ -14672,7 +14672,7 @@
         <v>559279</v>
       </c>
     </row>
-    <row r="124" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="124" spans="1:22" ht="19.95" customHeight="1">
       <c r="A124" s="1" t="s">
         <v>1562</v>
       </c>
@@ -14738,7 +14738,7 @@
         <v>559088</v>
       </c>
     </row>
-    <row r="125" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="125" spans="1:22" ht="19.95" customHeight="1">
       <c r="A125" s="1" t="s">
         <v>1563</v>
       </c>
@@ -14804,7 +14804,7 @@
         <v>559055</v>
       </c>
     </row>
-    <row r="126" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="126" spans="1:22" ht="19.95" customHeight="1">
       <c r="A126" s="1" t="s">
         <v>1564</v>
       </c>
@@ -14870,7 +14870,7 @@
         <v>559169</v>
       </c>
     </row>
-    <row r="127" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="127" spans="1:22" ht="19.95" customHeight="1">
       <c r="A127" s="1" t="s">
         <v>1565</v>
       </c>
@@ -14936,7 +14936,7 @@
         <v>559095</v>
       </c>
     </row>
-    <row r="128" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="128" spans="1:22" ht="19.95" customHeight="1">
       <c r="A128" s="1" t="s">
         <v>1566</v>
       </c>
@@ -15000,7 +15000,7 @@
         <v>559194</v>
       </c>
     </row>
-    <row r="129" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="129" spans="1:22" ht="19.95" customHeight="1">
       <c r="A129" s="1" t="s">
         <v>1567</v>
       </c>
@@ -15066,7 +15066,7 @@
         <v>559079</v>
       </c>
     </row>
-    <row r="130" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="130" spans="1:22" ht="19.95" customHeight="1">
       <c r="A130" s="1" t="s">
         <v>1568</v>
       </c>
@@ -15132,7 +15132,7 @@
         <v>559188</v>
       </c>
     </row>
-    <row r="131" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="131" spans="1:22" ht="19.95" customHeight="1">
       <c r="A131" s="1" t="s">
         <v>1569</v>
       </c>
@@ -15196,7 +15196,7 @@
         <v>559221</v>
       </c>
     </row>
-    <row r="132" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="132" spans="1:22" ht="19.95" customHeight="1">
       <c r="A132" s="1" t="s">
         <v>1570</v>
       </c>
@@ -15262,7 +15262,7 @@
         <v>559001</v>
       </c>
     </row>
-    <row r="133" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="133" spans="1:22" ht="19.95" customHeight="1">
       <c r="A133" s="1" t="s">
         <v>1571</v>
       </c>
@@ -15328,7 +15328,7 @@
         <v>559018</v>
       </c>
     </row>
-    <row r="134" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="134" spans="1:22" ht="19.95" customHeight="1">
       <c r="A134" s="1" t="s">
         <v>1572</v>
       </c>
@@ -15394,7 +15394,7 @@
         <v>559174</v>
       </c>
     </row>
-    <row r="135" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="135" spans="1:22" ht="19.95" customHeight="1">
       <c r="A135" s="1" t="s">
         <v>1573</v>
       </c>
@@ -15460,7 +15460,7 @@
         <v>559273</v>
       </c>
     </row>
-    <row r="136" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="136" spans="1:22" ht="19.95" customHeight="1">
       <c r="A136" s="1" t="s">
         <v>1574</v>
       </c>
@@ -15526,7 +15526,7 @@
         <v>559125</v>
       </c>
     </row>
-    <row r="137" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="137" spans="1:22" ht="19.95" customHeight="1">
       <c r="A137" s="1" t="s">
         <v>1575</v>
       </c>
@@ -15592,7 +15592,7 @@
         <v>559199</v>
       </c>
     </row>
-    <row r="138" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="138" spans="1:22" ht="19.95" customHeight="1">
       <c r="A138" s="1" t="s">
         <v>1576</v>
       </c>
@@ -15658,7 +15658,7 @@
         <v>559063</v>
       </c>
     </row>
-    <row r="139" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="139" spans="1:22" ht="19.95" customHeight="1">
       <c r="A139" s="1" t="s">
         <v>1577</v>
       </c>
@@ -15724,7 +15724,7 @@
         <v>559015</v>
       </c>
     </row>
-    <row r="140" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="140" spans="1:22" ht="19.95" customHeight="1">
       <c r="A140" s="1" t="s">
         <v>1578</v>
       </c>
@@ -15790,7 +15790,7 @@
         <v>559113</v>
       </c>
     </row>
-    <row r="141" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="141" spans="1:22" ht="19.95" customHeight="1">
       <c r="A141" s="1" t="s">
         <v>1579</v>
       </c>
@@ -15856,7 +15856,7 @@
         <v>559225</v>
       </c>
     </row>
-    <row r="142" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="142" spans="1:22" ht="19.95" customHeight="1">
       <c r="A142" s="1" t="s">
         <v>1580</v>
       </c>
@@ -15922,7 +15922,7 @@
         <v>559168</v>
       </c>
     </row>
-    <row r="143" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="143" spans="1:22" ht="19.95" customHeight="1">
       <c r="A143" s="1" t="s">
         <v>1581</v>
       </c>
@@ -15988,7 +15988,7 @@
         <v>559000</v>
       </c>
     </row>
-    <row r="144" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="144" spans="1:22" ht="19.95" customHeight="1">
       <c r="A144" s="1" t="s">
         <v>1582</v>
       </c>
@@ -16054,7 +16054,7 @@
         <v>559023</v>
       </c>
     </row>
-    <row r="145" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="145" spans="1:22" ht="19.95" customHeight="1">
       <c r="A145" s="1" t="s">
         <v>1583</v>
       </c>
@@ -16120,7 +16120,7 @@
         <v>559289</v>
       </c>
     </row>
-    <row r="146" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="146" spans="1:22" ht="19.95" customHeight="1">
       <c r="A146" s="1" t="s">
         <v>1584</v>
       </c>
@@ -16186,7 +16186,7 @@
         <v>559257</v>
       </c>
     </row>
-    <row r="147" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="147" spans="1:22" ht="19.95" customHeight="1">
       <c r="A147" s="1" t="s">
         <v>1585</v>
       </c>
@@ -16252,7 +16252,7 @@
         <v>559059</v>
       </c>
     </row>
-    <row r="148" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="148" spans="1:22" ht="19.95" customHeight="1">
       <c r="A148" s="1" t="s">
         <v>1586</v>
       </c>
@@ -16318,7 +16318,7 @@
         <v>559287</v>
       </c>
     </row>
-    <row r="149" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="149" spans="1:22" ht="19.95" customHeight="1">
       <c r="A149" s="1" t="s">
         <v>1587</v>
       </c>
@@ -16384,7 +16384,7 @@
         <v>559229</v>
       </c>
     </row>
-    <row r="150" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="150" spans="1:22" ht="19.95" customHeight="1">
       <c r="A150" s="1" t="s">
         <v>1588</v>
       </c>
@@ -16450,7 +16450,7 @@
         <v>559064</v>
       </c>
     </row>
-    <row r="151" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="151" spans="1:22" ht="19.95" customHeight="1">
       <c r="A151" s="1" t="s">
         <v>1589</v>
       </c>
@@ -16516,7 +16516,7 @@
         <v>559027</v>
       </c>
     </row>
-    <row r="152" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="152" spans="1:22" ht="19.95" customHeight="1">
       <c r="A152" s="1" t="s">
         <v>1590</v>
       </c>
@@ -16582,7 +16582,7 @@
         <v>559050</v>
       </c>
     </row>
-    <row r="153" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="153" spans="1:22" ht="19.95" customHeight="1">
       <c r="A153" s="1" t="s">
         <v>1591</v>
       </c>
@@ -16648,7 +16648,7 @@
         <v>559255</v>
       </c>
     </row>
-    <row r="154" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="154" spans="1:22" ht="19.95" customHeight="1">
       <c r="A154" s="1" t="s">
         <v>1592</v>
       </c>
@@ -16714,7 +16714,7 @@
         <v>559298</v>
       </c>
     </row>
-    <row r="155" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="155" spans="1:22" ht="19.95" customHeight="1">
       <c r="A155" s="1" t="s">
         <v>1593</v>
       </c>
@@ -16780,7 +16780,7 @@
         <v>559189</v>
       </c>
     </row>
-    <row r="156" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="156" spans="1:22" ht="19.95" customHeight="1">
       <c r="A156" s="1" t="s">
         <v>1594</v>
       </c>
@@ -16846,7 +16846,7 @@
         <v>559142</v>
       </c>
     </row>
-    <row r="157" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="157" spans="1:22" ht="19.95" customHeight="1">
       <c r="A157" s="1" t="s">
         <v>1595</v>
       </c>
@@ -16912,7 +16912,7 @@
         <v>559111</v>
       </c>
     </row>
-    <row r="158" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="158" spans="1:22" ht="19.95" customHeight="1">
       <c r="A158" s="1" t="s">
         <v>1596</v>
       </c>
@@ -16978,7 +16978,7 @@
         <v>559263</v>
       </c>
     </row>
-    <row r="159" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="159" spans="1:22" ht="19.95" customHeight="1">
       <c r="A159" s="1" t="s">
         <v>1597</v>
       </c>
@@ -17044,7 +17044,7 @@
         <v>559195</v>
       </c>
     </row>
-    <row r="160" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="160" spans="1:22" ht="19.95" customHeight="1">
       <c r="A160" s="1" t="s">
         <v>1598</v>
       </c>
@@ -17110,7 +17110,7 @@
         <v>559116</v>
       </c>
     </row>
-    <row r="161" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="161" spans="1:22" ht="19.95" customHeight="1">
       <c r="A161" s="1" t="s">
         <v>1599</v>
       </c>
@@ -17176,7 +17176,7 @@
         <v>559066</v>
       </c>
     </row>
-    <row r="162" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="162" spans="1:22" ht="19.95" customHeight="1">
       <c r="A162" s="1" t="s">
         <v>1600</v>
       </c>
@@ -17242,7 +17242,7 @@
         <v>559200</v>
       </c>
     </row>
-    <row r="163" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="163" spans="1:22" ht="19.95" customHeight="1">
       <c r="A163" s="1" t="s">
         <v>1601</v>
       </c>
@@ -17308,7 +17308,7 @@
         <v>559120</v>
       </c>
     </row>
-    <row r="164" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="164" spans="1:22" ht="19.95" customHeight="1">
       <c r="A164" s="1" t="s">
         <v>1602</v>
       </c>
@@ -17374,7 +17374,7 @@
         <v>559054</v>
       </c>
     </row>
-    <row r="165" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="165" spans="1:22" ht="19.95" customHeight="1">
       <c r="A165" s="1" t="s">
         <v>1603</v>
       </c>
@@ -17440,7 +17440,7 @@
         <v>559110</v>
       </c>
     </row>
-    <row r="166" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="166" spans="1:22" ht="19.95" customHeight="1">
       <c r="A166" s="1" t="s">
         <v>1604</v>
       </c>
@@ -17506,7 +17506,7 @@
         <v>559284</v>
       </c>
     </row>
-    <row r="167" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="167" spans="1:22" ht="19.95" customHeight="1">
       <c r="A167" s="1" t="s">
         <v>1605</v>
       </c>
@@ -17572,7 +17572,7 @@
         <v>559161</v>
       </c>
     </row>
-    <row r="168" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="168" spans="1:22" ht="19.95" customHeight="1">
       <c r="A168" s="1" t="s">
         <v>1606</v>
       </c>
@@ -17638,7 +17638,7 @@
         <v>559031</v>
       </c>
     </row>
-    <row r="169" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="169" spans="1:22" ht="19.95" customHeight="1">
       <c r="A169" s="1" t="s">
         <v>1607</v>
       </c>
@@ -17704,7 +17704,7 @@
         <v>559101</v>
       </c>
     </row>
-    <row r="170" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="170" spans="1:22" ht="19.95" customHeight="1">
       <c r="A170" s="1" t="s">
         <v>1608</v>
       </c>
@@ -17768,7 +17768,7 @@
         <v>559234</v>
       </c>
     </row>
-    <row r="171" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="171" spans="1:22" ht="19.95" customHeight="1">
       <c r="A171" s="1" t="s">
         <v>1609</v>
       </c>
@@ -17834,7 +17834,7 @@
         <v>559250</v>
       </c>
     </row>
-    <row r="172" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="172" spans="1:22" ht="19.95" customHeight="1">
       <c r="A172" s="1" t="s">
         <v>1610</v>
       </c>
@@ -17900,7 +17900,7 @@
         <v>559261</v>
       </c>
     </row>
-    <row r="173" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="173" spans="1:22" ht="19.95" customHeight="1">
       <c r="A173" s="1" t="s">
         <v>1611</v>
       </c>
@@ -17966,7 +17966,7 @@
         <v>559026</v>
       </c>
     </row>
-    <row r="174" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="174" spans="1:22" ht="19.95" customHeight="1">
       <c r="A174" s="1" t="s">
         <v>1612</v>
       </c>
@@ -18032,7 +18032,7 @@
         <v>559132</v>
       </c>
     </row>
-    <row r="175" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="175" spans="1:22" ht="19.95" customHeight="1">
       <c r="A175" s="1" t="s">
         <v>1613</v>
       </c>
@@ -18096,7 +18096,7 @@
         <v>559274</v>
       </c>
     </row>
-    <row r="176" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="176" spans="1:22" ht="19.95" customHeight="1">
       <c r="A176" s="1" t="s">
         <v>1614</v>
       </c>
@@ -18162,7 +18162,7 @@
         <v>559130</v>
       </c>
     </row>
-    <row r="177" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="177" spans="1:22" ht="19.95" customHeight="1">
       <c r="A177" s="1" t="s">
         <v>1615</v>
       </c>
@@ -18228,7 +18228,7 @@
         <v>559247</v>
       </c>
     </row>
-    <row r="178" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="178" spans="1:22" ht="19.95" customHeight="1">
       <c r="A178" s="1" t="s">
         <v>1616</v>
       </c>
@@ -18294,7 +18294,7 @@
         <v>559203</v>
       </c>
     </row>
-    <row r="179" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="179" spans="1:22" ht="19.95" customHeight="1">
       <c r="A179" s="1" t="s">
         <v>1617</v>
       </c>
@@ -18360,7 +18360,7 @@
         <v>559237</v>
       </c>
     </row>
-    <row r="180" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="180" spans="1:22" ht="19.95" customHeight="1">
       <c r="A180" s="1" t="s">
         <v>1618</v>
       </c>
@@ -18426,7 +18426,7 @@
         <v>559117</v>
       </c>
     </row>
-    <row r="181" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="181" spans="1:22" ht="19.95" customHeight="1">
       <c r="A181" s="1" t="s">
         <v>1619</v>
       </c>
@@ -18492,7 +18492,7 @@
         <v>559005</v>
       </c>
     </row>
-    <row r="182" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="182" spans="1:22" ht="19.95" customHeight="1">
       <c r="A182" s="1" t="s">
         <v>1620</v>
       </c>
@@ -18558,7 +18558,7 @@
         <v>559072</v>
       </c>
     </row>
-    <row r="183" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="183" spans="1:22" ht="19.95" customHeight="1">
       <c r="A183" s="1" t="s">
         <v>1621</v>
       </c>
@@ -18624,7 +18624,7 @@
         <v>559281</v>
       </c>
     </row>
-    <row r="184" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="184" spans="1:22" ht="19.95" customHeight="1">
       <c r="A184" s="1" t="s">
         <v>1622</v>
       </c>
@@ -18690,7 +18690,7 @@
         <v>559133</v>
       </c>
     </row>
-    <row r="185" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="185" spans="1:22" ht="19.95" customHeight="1">
       <c r="A185" s="1" t="s">
         <v>1623</v>
       </c>
@@ -18756,7 +18756,7 @@
         <v>559033</v>
       </c>
     </row>
-    <row r="186" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="186" spans="1:22" ht="19.95" customHeight="1">
       <c r="A186" s="1" t="s">
         <v>1624</v>
       </c>
@@ -18822,7 +18822,7 @@
         <v>559202</v>
       </c>
     </row>
-    <row r="187" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="187" spans="1:22" ht="19.95" customHeight="1">
       <c r="A187" s="1" t="s">
         <v>1625</v>
       </c>
@@ -18888,7 +18888,7 @@
         <v>559267</v>
       </c>
     </row>
-    <row r="188" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="188" spans="1:22" ht="19.95" customHeight="1">
       <c r="A188" s="1" t="s">
         <v>1626</v>
       </c>
@@ -18954,7 +18954,7 @@
         <v>559043</v>
       </c>
     </row>
-    <row r="189" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="189" spans="1:22" ht="19.95" customHeight="1">
       <c r="A189" s="1" t="s">
         <v>1627</v>
       </c>
@@ -19020,7 +19020,7 @@
         <v>559104</v>
       </c>
     </row>
-    <row r="190" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="190" spans="1:22" ht="19.95" customHeight="1">
       <c r="A190" s="1" t="s">
         <v>1628</v>
       </c>
@@ -19086,7 +19086,7 @@
         <v>559241</v>
       </c>
     </row>
-    <row r="191" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="191" spans="1:22" ht="19.95" customHeight="1">
       <c r="A191" s="1" t="s">
         <v>1629</v>
       </c>
@@ -19152,7 +19152,7 @@
         <v>559166</v>
       </c>
     </row>
-    <row r="192" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="192" spans="1:22" ht="19.95" customHeight="1">
       <c r="A192" s="1" t="s">
         <v>1630</v>
       </c>
@@ -19218,7 +19218,7 @@
         <v>559163</v>
       </c>
     </row>
-    <row r="193" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="193" spans="1:22" ht="19.95" customHeight="1">
       <c r="A193" s="1" t="s">
         <v>1631</v>
       </c>
@@ -19284,7 +19284,7 @@
         <v>559058</v>
       </c>
     </row>
-    <row r="194" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="194" spans="1:22" ht="19.95" customHeight="1">
       <c r="A194" s="1" t="s">
         <v>1632</v>
       </c>
@@ -19350,7 +19350,7 @@
         <v>559090</v>
       </c>
     </row>
-    <row r="195" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="195" spans="1:22" ht="19.95" customHeight="1">
       <c r="A195" s="1" t="s">
         <v>1633</v>
       </c>
@@ -19416,7 +19416,7 @@
         <v>559118</v>
       </c>
     </row>
-    <row r="196" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="196" spans="1:22" ht="19.95" customHeight="1">
       <c r="A196" s="1" t="s">
         <v>1634</v>
       </c>
@@ -19482,7 +19482,7 @@
         <v>559246</v>
       </c>
     </row>
-    <row r="197" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="197" spans="1:22" ht="19.95" customHeight="1">
       <c r="A197" s="1" t="s">
         <v>1635</v>
       </c>
@@ -19548,7 +19548,7 @@
         <v>559134</v>
       </c>
     </row>
-    <row r="198" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="198" spans="1:22" ht="19.95" customHeight="1">
       <c r="A198" s="1" t="s">
         <v>1636</v>
       </c>
@@ -19614,7 +19614,7 @@
         <v>559280</v>
       </c>
     </row>
-    <row r="199" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="199" spans="1:22" ht="19.95" customHeight="1">
       <c r="A199" s="1" t="s">
         <v>1637</v>
       </c>
@@ -19680,7 +19680,7 @@
         <v>559112</v>
       </c>
     </row>
-    <row r="200" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="200" spans="1:22" ht="19.95" customHeight="1">
       <c r="A200" s="1" t="s">
         <v>1638</v>
       </c>
@@ -19746,7 +19746,7 @@
         <v>559070</v>
       </c>
     </row>
-    <row r="201" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="201" spans="1:22" ht="19.95" customHeight="1">
       <c r="A201" s="1" t="s">
         <v>1639</v>
       </c>
@@ -19812,7 +19812,7 @@
         <v>559210</v>
       </c>
     </row>
-    <row r="202" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="202" spans="1:22" ht="19.95" customHeight="1">
       <c r="A202" s="1" t="s">
         <v>1640</v>
       </c>
@@ -19878,7 +19878,7 @@
         <v>559292</v>
       </c>
     </row>
-    <row r="203" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="203" spans="1:22" ht="19.95" customHeight="1">
       <c r="A203" s="1" t="s">
         <v>1641</v>
       </c>
@@ -19944,7 +19944,7 @@
         <v>559164</v>
       </c>
     </row>
-    <row r="204" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="204" spans="1:22" ht="19.95" customHeight="1">
       <c r="A204" s="1" t="s">
         <v>1642</v>
       </c>
@@ -20010,7 +20010,7 @@
         <v>559269</v>
       </c>
     </row>
-    <row r="205" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="205" spans="1:22" ht="19.95" customHeight="1">
       <c r="A205" s="1" t="s">
         <v>1643</v>
       </c>
@@ -20076,7 +20076,7 @@
         <v>559061</v>
       </c>
     </row>
-    <row r="206" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="206" spans="1:22" ht="19.95" customHeight="1">
       <c r="A206" s="1" t="s">
         <v>1644</v>
       </c>
@@ -20142,7 +20142,7 @@
         <v>559122</v>
       </c>
     </row>
-    <row r="207" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="207" spans="1:22" ht="19.95" customHeight="1">
       <c r="A207" s="1" t="s">
         <v>1645</v>
       </c>
@@ -20208,7 +20208,7 @@
         <v>559205</v>
       </c>
     </row>
-    <row r="208" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="208" spans="1:22" ht="19.95" customHeight="1">
       <c r="A208" s="1" t="s">
         <v>1646</v>
       </c>
@@ -20274,7 +20274,7 @@
         <v>559173</v>
       </c>
     </row>
-    <row r="209" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="209" spans="1:22" ht="19.95" customHeight="1">
       <c r="A209" s="1" t="s">
         <v>1647</v>
       </c>
@@ -20340,7 +20340,7 @@
         <v>559131</v>
       </c>
     </row>
-    <row r="210" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="210" spans="1:22" ht="19.95" customHeight="1">
       <c r="A210" s="1" t="s">
         <v>1648</v>
       </c>
@@ -20406,7 +20406,7 @@
         <v>559262</v>
       </c>
     </row>
-    <row r="211" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="211" spans="1:22" ht="19.95" customHeight="1">
       <c r="A211" s="1" t="s">
         <v>1649</v>
       </c>
@@ -20472,7 +20472,7 @@
         <v>559089</v>
       </c>
     </row>
-    <row r="212" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="212" spans="1:22" ht="19.95" customHeight="1">
       <c r="A212" s="1" t="s">
         <v>1650</v>
       </c>
@@ -20538,7 +20538,7 @@
         <v>559037</v>
       </c>
     </row>
-    <row r="213" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="213" spans="1:22" ht="19.95" customHeight="1">
       <c r="A213" s="1" t="s">
         <v>1651</v>
       </c>
@@ -20604,7 +20604,7 @@
         <v>559013</v>
       </c>
     </row>
-    <row r="214" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="214" spans="1:22" ht="19.95" customHeight="1">
       <c r="A214" s="1" t="s">
         <v>1652</v>
       </c>
@@ -20670,7 +20670,7 @@
         <v>559083</v>
       </c>
     </row>
-    <row r="215" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="215" spans="1:22" ht="19.95" customHeight="1">
       <c r="A215" s="1" t="s">
         <v>1653</v>
       </c>
@@ -20736,7 +20736,7 @@
         <v>559077</v>
       </c>
     </row>
-    <row r="216" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="216" spans="1:22" ht="19.95" customHeight="1">
       <c r="A216" s="1" t="s">
         <v>1654</v>
       </c>
@@ -20802,7 +20802,7 @@
         <v>559196</v>
       </c>
     </row>
-    <row r="217" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="217" spans="1:22" ht="19.95" customHeight="1">
       <c r="A217" s="1" t="s">
         <v>1655</v>
       </c>
@@ -20868,7 +20868,7 @@
         <v>559191</v>
       </c>
     </row>
-    <row r="218" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="218" spans="1:22" ht="19.95" customHeight="1">
       <c r="A218" s="1" t="s">
         <v>1656</v>
       </c>
@@ -20934,7 +20934,7 @@
         <v>559193</v>
       </c>
     </row>
-    <row r="219" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="219" spans="1:22" ht="19.95" customHeight="1">
       <c r="A219" s="1" t="s">
         <v>1657</v>
       </c>
@@ -20998,7 +20998,7 @@
         <v>559254</v>
       </c>
     </row>
-    <row r="220" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="220" spans="1:22" ht="19.95" customHeight="1">
       <c r="A220" s="1" t="s">
         <v>1658</v>
       </c>
@@ -21064,7 +21064,7 @@
         <v>559092</v>
       </c>
     </row>
-    <row r="221" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="221" spans="1:22" ht="19.95" customHeight="1">
       <c r="A221" s="1" t="s">
         <v>1659</v>
       </c>
@@ -21130,7 +21130,7 @@
         <v>559137</v>
       </c>
     </row>
-    <row r="222" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="222" spans="1:22" ht="19.95" customHeight="1">
       <c r="A222" s="1" t="s">
         <v>1660</v>
       </c>
@@ -21196,7 +21196,7 @@
         <v>559207</v>
       </c>
     </row>
-    <row r="223" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="223" spans="1:22" ht="19.95" customHeight="1">
       <c r="A223" s="1" t="s">
         <v>1661</v>
       </c>
@@ -21262,7 +21262,7 @@
         <v>559190</v>
       </c>
     </row>
-    <row r="224" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="224" spans="1:22" ht="19.95" customHeight="1">
       <c r="A224" s="1" t="s">
         <v>1662</v>
       </c>
@@ -21328,7 +21328,7 @@
         <v>559108</v>
       </c>
     </row>
-    <row r="225" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="225" spans="1:22" ht="19.95" customHeight="1">
       <c r="A225" s="1" t="s">
         <v>1663</v>
       </c>
@@ -21394,7 +21394,7 @@
         <v>559040</v>
       </c>
     </row>
-    <row r="226" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="226" spans="1:22" ht="19.95" customHeight="1">
       <c r="A226" s="1" t="s">
         <v>1664</v>
       </c>
@@ -21460,7 +21460,7 @@
         <v>559076</v>
       </c>
     </row>
-    <row r="227" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="227" spans="1:22" ht="19.95" customHeight="1">
       <c r="A227" s="1" t="s">
         <v>1665</v>
       </c>
@@ -21526,7 +21526,7 @@
         <v>559266</v>
       </c>
     </row>
-    <row r="228" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="228" spans="1:22" ht="19.95" customHeight="1">
       <c r="A228" s="1" t="s">
         <v>1666</v>
       </c>
@@ -21592,7 +21592,7 @@
         <v>559006</v>
       </c>
     </row>
-    <row r="229" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="229" spans="1:22" ht="19.95" customHeight="1">
       <c r="A229" s="1" t="s">
         <v>1667</v>
       </c>
@@ -21658,7 +21658,7 @@
         <v>559094</v>
       </c>
     </row>
-    <row r="230" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="230" spans="1:22" ht="19.95" customHeight="1">
       <c r="A230" s="1" t="s">
         <v>1668</v>
       </c>
@@ -21724,7 +21724,7 @@
         <v>559068</v>
       </c>
     </row>
-    <row r="231" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="231" spans="1:22" ht="19.95" customHeight="1">
       <c r="A231" s="1" t="s">
         <v>1669</v>
       </c>
@@ -21790,7 +21790,7 @@
         <v>559078</v>
       </c>
     </row>
-    <row r="232" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="232" spans="1:22" ht="19.95" customHeight="1">
       <c r="A232" s="1" t="s">
         <v>1670</v>
       </c>
@@ -21856,7 +21856,7 @@
         <v>559299</v>
       </c>
     </row>
-    <row r="233" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="233" spans="1:22" ht="19.95" customHeight="1">
       <c r="A233" s="1" t="s">
         <v>1671</v>
       </c>
@@ -21922,7 +21922,7 @@
         <v>559197</v>
       </c>
     </row>
-    <row r="234" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="234" spans="1:22" ht="19.95" customHeight="1">
       <c r="A234" s="1" t="s">
         <v>1672</v>
       </c>
@@ -21988,7 +21988,7 @@
         <v>559268</v>
       </c>
     </row>
-    <row r="235" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="235" spans="1:22" ht="19.95" customHeight="1">
       <c r="A235" s="1" t="s">
         <v>1673</v>
       </c>
@@ -22054,7 +22054,7 @@
         <v>559217</v>
       </c>
     </row>
-    <row r="236" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="236" spans="1:22" ht="19.95" customHeight="1">
       <c r="A236" s="1" t="s">
         <v>1674</v>
       </c>
@@ -22120,7 +22120,7 @@
         <v>559034</v>
       </c>
     </row>
-    <row r="237" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="237" spans="1:22" ht="19.95" customHeight="1">
       <c r="A237" s="1" t="s">
         <v>1675</v>
       </c>
@@ -22186,7 +22186,7 @@
         <v>559107</v>
       </c>
     </row>
-    <row r="238" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="238" spans="1:22" ht="19.95" customHeight="1">
       <c r="A238" s="1" t="s">
         <v>1676</v>
       </c>
@@ -22252,7 +22252,7 @@
         <v>559075</v>
       </c>
     </row>
-    <row r="239" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="239" spans="1:22" ht="19.95" customHeight="1">
       <c r="A239" s="1" t="s">
         <v>1677</v>
       </c>
@@ -22318,7 +22318,7 @@
         <v>559053</v>
       </c>
     </row>
-    <row r="240" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="240" spans="1:22" ht="19.95" customHeight="1">
       <c r="A240" s="1" t="s">
         <v>1678</v>
       </c>
@@ -22384,7 +22384,7 @@
         <v>559123</v>
       </c>
     </row>
-    <row r="241" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="241" spans="1:22" ht="19.95" customHeight="1">
       <c r="A241" s="1" t="s">
         <v>1679</v>
       </c>
@@ -22450,7 +22450,7 @@
         <v>559100</v>
       </c>
     </row>
-    <row r="242" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="242" spans="1:22" ht="19.95" customHeight="1">
       <c r="A242" s="1" t="s">
         <v>1680</v>
       </c>
@@ -22516,7 +22516,7 @@
         <v>559146</v>
       </c>
     </row>
-    <row r="243" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="243" spans="1:22" ht="19.95" customHeight="1">
       <c r="A243" s="1" t="s">
         <v>1681</v>
       </c>
@@ -22582,7 +22582,7 @@
         <v>559158</v>
       </c>
     </row>
-    <row r="244" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="244" spans="1:22" ht="19.95" customHeight="1">
       <c r="A244" s="1" t="s">
         <v>1682</v>
       </c>
@@ -22648,7 +22648,7 @@
         <v>559086</v>
       </c>
     </row>
-    <row r="245" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="245" spans="1:22" ht="19.95" customHeight="1">
       <c r="A245" s="1" t="s">
         <v>1683</v>
       </c>
@@ -22714,7 +22714,7 @@
         <v>559030</v>
       </c>
     </row>
-    <row r="246" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="246" spans="1:22" ht="19.95" customHeight="1">
       <c r="A246" s="1" t="s">
         <v>1684</v>
       </c>
@@ -22780,7 +22780,7 @@
         <v>559232</v>
       </c>
     </row>
-    <row r="247" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="247" spans="1:22" ht="19.95" customHeight="1">
       <c r="A247" s="1" t="s">
         <v>1685</v>
       </c>
@@ -22846,7 +22846,7 @@
         <v>559224</v>
       </c>
     </row>
-    <row r="248" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="248" spans="1:22" ht="19.95" customHeight="1">
       <c r="A248" s="1" t="s">
         <v>1686</v>
       </c>
@@ -22912,7 +22912,7 @@
         <v>559297</v>
       </c>
     </row>
-    <row r="249" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="249" spans="1:22" ht="19.95" customHeight="1">
       <c r="A249" s="1" t="s">
         <v>1687</v>
       </c>
@@ -22978,7 +22978,7 @@
         <v>559282</v>
       </c>
     </row>
-    <row r="250" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="250" spans="1:22" ht="19.95" customHeight="1">
       <c r="A250" s="1" t="s">
         <v>1688</v>
       </c>
@@ -23042,7 +23042,7 @@
         <v>559109</v>
       </c>
     </row>
-    <row r="251" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="251" spans="1:22" ht="19.95" customHeight="1">
       <c r="A251" s="1" t="s">
         <v>1689</v>
       </c>
@@ -23108,7 +23108,7 @@
         <v>559028</v>
       </c>
     </row>
-    <row r="252" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="252" spans="1:22" ht="19.95" customHeight="1">
       <c r="A252" s="1" t="s">
         <v>1690</v>
       </c>
@@ -23174,7 +23174,7 @@
         <v>559129</v>
       </c>
     </row>
-    <row r="253" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="253" spans="1:22" ht="19.95" customHeight="1">
       <c r="A253" s="1" t="s">
         <v>1691</v>
       </c>
@@ -23240,7 +23240,7 @@
         <v>559243</v>
       </c>
     </row>
-    <row r="254" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="254" spans="1:22" ht="19.95" customHeight="1">
       <c r="A254" s="1" t="s">
         <v>1692</v>
       </c>
@@ -23306,7 +23306,7 @@
         <v>559219</v>
       </c>
     </row>
-    <row r="255" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="255" spans="1:22" ht="19.95" customHeight="1">
       <c r="A255" s="1" t="s">
         <v>1693</v>
       </c>
@@ -23372,7 +23372,7 @@
         <v>559235</v>
       </c>
     </row>
-    <row r="256" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="256" spans="1:22" ht="19.95" customHeight="1">
       <c r="A256" s="1" t="s">
         <v>1694</v>
       </c>
@@ -23438,7 +23438,7 @@
         <v>559041</v>
       </c>
     </row>
-    <row r="257" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="257" spans="1:22" ht="19.95" customHeight="1">
       <c r="A257" s="1" t="s">
         <v>1695</v>
       </c>
@@ -23504,7 +23504,7 @@
         <v>559029</v>
       </c>
     </row>
-    <row r="258" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="258" spans="1:22" ht="19.95" customHeight="1">
       <c r="A258" s="1" t="s">
         <v>1696</v>
       </c>
@@ -23570,7 +23570,7 @@
         <v>559048</v>
       </c>
     </row>
-    <row r="259" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="259" spans="1:22" ht="19.95" customHeight="1">
       <c r="A259" s="1" t="s">
         <v>1697</v>
       </c>
@@ -23636,7 +23636,7 @@
         <v>559007</v>
       </c>
     </row>
-    <row r="260" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="260" spans="1:22" ht="19.95" customHeight="1">
       <c r="A260" s="1" t="s">
         <v>1698</v>
       </c>
@@ -23702,7 +23702,7 @@
         <v>559147</v>
       </c>
     </row>
-    <row r="261" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="261" spans="1:22" ht="19.95" customHeight="1">
       <c r="A261" s="1" t="s">
         <v>1699</v>
       </c>
@@ -23768,7 +23768,7 @@
         <v>559073</v>
       </c>
     </row>
-    <row r="262" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="262" spans="1:22" ht="19.95" customHeight="1">
       <c r="A262" s="1" t="s">
         <v>1700</v>
       </c>
@@ -23834,7 +23834,7 @@
         <v>559119</v>
       </c>
     </row>
-    <row r="263" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="263" spans="1:22" ht="19.95" customHeight="1">
       <c r="A263" s="1" t="s">
         <v>1701</v>
       </c>
@@ -23900,7 +23900,7 @@
         <v>559211</v>
       </c>
     </row>
-    <row r="264" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="264" spans="1:22" ht="19.95" customHeight="1">
       <c r="A264" s="1" t="s">
         <v>1702</v>
       </c>
@@ -23966,7 +23966,7 @@
         <v>559045</v>
       </c>
     </row>
-    <row r="265" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="265" spans="1:22" ht="19.95" customHeight="1">
       <c r="A265" s="1" t="s">
         <v>1703</v>
       </c>
@@ -24032,7 +24032,7 @@
         <v>559223</v>
       </c>
     </row>
-    <row r="266" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="266" spans="1:22" ht="19.95" customHeight="1">
       <c r="A266" s="1" t="s">
         <v>1704</v>
       </c>
@@ -24098,7 +24098,7 @@
         <v>559240</v>
       </c>
     </row>
-    <row r="267" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="267" spans="1:22" ht="19.95" customHeight="1">
       <c r="A267" s="1" t="s">
         <v>1705</v>
       </c>
@@ -24164,7 +24164,7 @@
         <v>559081</v>
       </c>
     </row>
-    <row r="268" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="268" spans="1:22" ht="19.95" customHeight="1">
       <c r="A268" s="1" t="s">
         <v>1706</v>
       </c>
@@ -24230,7 +24230,7 @@
         <v>559049</v>
       </c>
     </row>
-    <row r="269" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="269" spans="1:22" ht="19.95" customHeight="1">
       <c r="A269" s="1" t="s">
         <v>1707</v>
       </c>
@@ -24296,7 +24296,7 @@
         <v>559249</v>
       </c>
     </row>
-    <row r="270" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="270" spans="1:22" ht="19.95" customHeight="1">
       <c r="A270" s="1" t="s">
         <v>1708</v>
       </c>
@@ -24362,7 +24362,7 @@
         <v>559181</v>
       </c>
     </row>
-    <row r="271" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="271" spans="1:22" ht="19.95" customHeight="1">
       <c r="A271" s="1" t="s">
         <v>1709</v>
       </c>
@@ -24428,7 +24428,7 @@
         <v>559022</v>
       </c>
     </row>
-    <row r="272" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="272" spans="1:22" ht="19.95" customHeight="1">
       <c r="A272" s="1" t="s">
         <v>1710</v>
       </c>
@@ -24494,7 +24494,7 @@
         <v>559206</v>
       </c>
     </row>
-    <row r="273" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="273" spans="1:22" ht="19.95" customHeight="1">
       <c r="A273" s="1" t="s">
         <v>1711</v>
       </c>
@@ -24560,7 +24560,7 @@
         <v>559019</v>
       </c>
     </row>
-    <row r="274" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="274" spans="1:22" ht="19.95" customHeight="1">
       <c r="A274" s="1" t="s">
         <v>1712</v>
       </c>
@@ -24626,7 +24626,7 @@
         <v>559178</v>
       </c>
     </row>
-    <row r="275" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="275" spans="1:22" ht="19.95" customHeight="1">
       <c r="A275" s="1" t="s">
         <v>1713</v>
       </c>
@@ -24692,7 +24692,7 @@
         <v>559214</v>
       </c>
     </row>
-    <row r="276" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="276" spans="1:22" ht="19.95" customHeight="1">
       <c r="A276" s="1" t="s">
         <v>1714</v>
       </c>
@@ -24758,7 +24758,7 @@
         <v>559008</v>
       </c>
     </row>
-    <row r="277" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="277" spans="1:22" ht="19.95" customHeight="1">
       <c r="A277" s="1" t="s">
         <v>1715</v>
       </c>
@@ -24824,7 +24824,7 @@
         <v>559141</v>
       </c>
     </row>
-    <row r="278" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="278" spans="1:22" ht="19.95" customHeight="1">
       <c r="A278" s="1" t="s">
         <v>1716</v>
       </c>
@@ -24890,7 +24890,7 @@
         <v>559286</v>
       </c>
     </row>
-    <row r="279" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="279" spans="1:22" ht="19.95" customHeight="1">
       <c r="A279" s="1" t="s">
         <v>1717</v>
       </c>
@@ -24956,7 +24956,7 @@
         <v>559208</v>
       </c>
     </row>
-    <row r="280" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="280" spans="1:22" ht="19.95" customHeight="1">
       <c r="A280" s="1" t="s">
         <v>1718</v>
       </c>
@@ -25022,7 +25022,7 @@
         <v>559003</v>
       </c>
     </row>
-    <row r="281" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="281" spans="1:22" ht="19.95" customHeight="1">
       <c r="A281" s="1" t="s">
         <v>1719</v>
       </c>
@@ -25088,7 +25088,7 @@
         <v>559149</v>
       </c>
     </row>
-    <row r="282" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="282" spans="1:22" ht="19.95" customHeight="1">
       <c r="A282" s="1" t="s">
         <v>1720</v>
       </c>
@@ -25154,7 +25154,7 @@
         <v>559215</v>
       </c>
     </row>
-    <row r="283" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="283" spans="1:22" ht="19.95" customHeight="1">
       <c r="A283" s="1" t="s">
         <v>1721</v>
       </c>
@@ -25220,7 +25220,7 @@
         <v>559192</v>
       </c>
     </row>
-    <row r="284" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="284" spans="1:22" ht="19.95" customHeight="1">
       <c r="A284" s="1" t="s">
         <v>1722</v>
       </c>
@@ -25286,7 +25286,7 @@
         <v>559035</v>
       </c>
     </row>
-    <row r="285" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="285" spans="1:22" ht="19.95" customHeight="1">
       <c r="A285" s="1" t="s">
         <v>1723</v>
       </c>
@@ -25352,7 +25352,7 @@
         <v>559144</v>
       </c>
     </row>
-    <row r="286" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="286" spans="1:22" ht="19.95" customHeight="1">
       <c r="A286" s="1" t="s">
         <v>1724</v>
       </c>
@@ -25418,7 +25418,7 @@
         <v>559222</v>
       </c>
     </row>
-    <row r="287" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="287" spans="1:22" ht="19.95" customHeight="1">
       <c r="A287" s="1" t="s">
         <v>1725</v>
       </c>
@@ -25484,7 +25484,7 @@
         <v>559253</v>
       </c>
     </row>
-    <row r="288" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="288" spans="1:22" ht="19.95" customHeight="1">
       <c r="A288" s="1" t="s">
         <v>1726</v>
       </c>
@@ -25550,7 +25550,7 @@
         <v>559128</v>
       </c>
     </row>
-    <row r="289" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="289" spans="1:22" ht="19.95" customHeight="1">
       <c r="A289" s="1" t="s">
         <v>1727</v>
       </c>
@@ -25616,7 +25616,7 @@
         <v>559153</v>
       </c>
     </row>
-    <row r="290" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="290" spans="1:22" ht="19.95" customHeight="1">
       <c r="A290" s="1" t="s">
         <v>1728</v>
       </c>
@@ -25682,7 +25682,7 @@
         <v>559172</v>
       </c>
     </row>
-    <row r="291" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="291" spans="1:22" ht="19.95" customHeight="1">
       <c r="A291" s="1" t="s">
         <v>1729</v>
       </c>
@@ -25748,7 +25748,7 @@
         <v>559228</v>
       </c>
     </row>
-    <row r="292" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="292" spans="1:22" ht="19.95" customHeight="1">
       <c r="A292" s="1" t="s">
         <v>1730</v>
       </c>
@@ -25814,7 +25814,7 @@
         <v>559285</v>
       </c>
     </row>
-    <row r="293" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="293" spans="1:22" ht="19.95" customHeight="1">
       <c r="A293" s="1" t="s">
         <v>1731</v>
       </c>
@@ -25880,7 +25880,7 @@
         <v>559162</v>
       </c>
     </row>
-    <row r="294" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="294" spans="1:22" ht="19.95" customHeight="1">
       <c r="A294" s="1" t="s">
         <v>1732</v>
       </c>
@@ -25946,7 +25946,7 @@
         <v>559143</v>
       </c>
     </row>
-    <row r="295" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="295" spans="1:22" ht="19.95" customHeight="1">
       <c r="A295" s="1" t="s">
         <v>1733</v>
       </c>
@@ -26012,7 +26012,7 @@
         <v>559175</v>
       </c>
     </row>
-    <row r="296" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="296" spans="1:22" ht="19.95" customHeight="1">
       <c r="A296" s="1" t="s">
         <v>1734</v>
       </c>
@@ -26078,7 +26078,7 @@
         <v>559242</v>
       </c>
     </row>
-    <row r="297" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="297" spans="1:22" ht="19.95" customHeight="1">
       <c r="A297" s="1" t="s">
         <v>1735</v>
       </c>
@@ -26144,7 +26144,7 @@
         <v>559185</v>
       </c>
     </row>
-    <row r="298" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="298" spans="1:22" ht="19.95" customHeight="1">
       <c r="A298" s="1" t="s">
         <v>1736</v>
       </c>
@@ -26210,7 +26210,7 @@
         <v>559170</v>
       </c>
     </row>
-    <row r="299" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="299" spans="1:22" ht="19.95" customHeight="1">
       <c r="A299" s="1" t="s">
         <v>1737</v>
       </c>
@@ -26276,7 +26276,7 @@
         <v>559180</v>
       </c>
     </row>
-    <row r="300" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="300" spans="1:22" ht="19.95" customHeight="1">
       <c r="A300" s="1" t="s">
         <v>1738</v>
       </c>
@@ -26342,7 +26342,7 @@
         <v>559039</v>
       </c>
     </row>
-    <row r="301" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="301" spans="1:22" ht="19.95" customHeight="1">
       <c r="A301" s="1" t="s">
         <v>1739</v>
       </c>
@@ -26408,7 +26408,7 @@
         <v>559213</v>
       </c>
     </row>
-    <row r="302" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="302" spans="1:22" ht="19.95" customHeight="1">
       <c r="A302" s="1" t="s">
         <v>1740</v>
       </c>
@@ -26474,7 +26474,7 @@
         <v>559252</v>
       </c>
     </row>
-    <row r="303" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="303" spans="1:22" ht="19.95" customHeight="1">
       <c r="B303" s="7"/>
       <c r="C303" s="8"/>
       <c r="I303" s="8"/>
@@ -26485,7 +26485,7 @@
       <c r="T303" s="8"/>
       <c r="U303" s="10"/>
     </row>
-    <row r="304" spans="1:22" ht="19.899999999999999" customHeight="1">
+    <row r="304" spans="1:22" ht="19.95" customHeight="1">
       <c r="C304" s="8"/>
       <c r="J304" s="8"/>
       <c r="Q304" s="9"/>

</xml_diff>